<commit_message>
bunch of changes, incl adding rugby post
</commit_message>
<xml_diff>
--- a/_posts/2020-11-17-is-the-government-as-safe-as-houses/data/rbnz_wholesale_rates.xlsx
+++ b/_posts/2020-11-17-is-the-government-as-safe-as-houses/data/rbnz_wholesale_rates.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\rbnz\dfs\homedrives\kimm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\rbnz\dfs\homedrives\suppanm\Desktop\CheckingTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10350" windowHeight="10830"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -590,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O435"/>
+  <dimension ref="A1:O452"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
@@ -15354,6 +15354,724 @@
       </c>
       <c r="O435" s="7">
         <v>-0.15</v>
+      </c>
+    </row>
+    <row r="436" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A436" s="10">
+        <v>44165</v>
+      </c>
+      <c r="B436" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C436" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="D436" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="E436" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="F436" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="G436" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="H436" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="I436" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="J436" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="L436" s="8">
+        <v>-0.53</v>
+      </c>
+      <c r="M436" s="8">
+        <v>-0.41</v>
+      </c>
+      <c r="N436" s="8">
+        <v>-0.24</v>
+      </c>
+      <c r="O436" s="7">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="437" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A437" s="10">
+        <v>44196</v>
+      </c>
+      <c r="B437" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C437" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="D437" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="E437" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="F437" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="H437" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="I437" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="J437" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="L437" s="8">
+        <v>-0.51</v>
+      </c>
+      <c r="M437" s="8">
+        <v>-0.35</v>
+      </c>
+      <c r="N437" s="8">
+        <v>-0.09</v>
+      </c>
+      <c r="O437" s="7">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="438" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A438" s="10">
+        <v>44227</v>
+      </c>
+      <c r="B438" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C438" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="D438" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="E438" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="F438" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H438" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="I438" s="8">
+        <v>0.39</v>
+      </c>
+      <c r="J438" s="8">
+        <v>1.04</v>
+      </c>
+      <c r="L438" s="8">
+        <v>-0.62</v>
+      </c>
+      <c r="M438" s="8">
+        <v>-0.42</v>
+      </c>
+      <c r="N438" s="8">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="O438" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="439" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A439" s="10">
+        <v>44255</v>
+      </c>
+      <c r="B439" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C439" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="D439" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="E439" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="F439" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H439" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="I439" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="J439" s="8">
+        <v>1.46</v>
+      </c>
+      <c r="L439" s="8">
+        <v>-0.73</v>
+      </c>
+      <c r="M439" s="8">
+        <v>-0.31</v>
+      </c>
+      <c r="N439" s="8">
+        <v>0.13</v>
+      </c>
+      <c r="O439" s="7">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="440" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A440" s="10">
+        <v>44286</v>
+      </c>
+      <c r="B440" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C440" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="D440" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="E440" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F440" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="H440" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="I440" s="8">
+        <v>1.03</v>
+      </c>
+      <c r="J440" s="8">
+        <v>1.76</v>
+      </c>
+      <c r="L440" s="8">
+        <v>-0.86</v>
+      </c>
+      <c r="M440" s="8">
+        <v>-0.22</v>
+      </c>
+      <c r="N440" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="O440" s="7">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="441" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A441" s="10">
+        <v>44316</v>
+      </c>
+      <c r="B441" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C441" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="D441" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="E441" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="F441" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="H441" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="I441" s="8">
+        <v>0.88</v>
+      </c>
+      <c r="J441" s="8">
+        <v>1.68</v>
+      </c>
+      <c r="L441" s="8">
+        <v>-1</v>
+      </c>
+      <c r="M441" s="8">
+        <v>-0.2</v>
+      </c>
+      <c r="N441" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="O441" s="7">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="442" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A442" s="10">
+        <v>44347</v>
+      </c>
+      <c r="B442" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C442" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="D442" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="E442" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="F442" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="H442" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="I442" s="8">
+        <v>1.03</v>
+      </c>
+      <c r="J442" s="8">
+        <v>1.81</v>
+      </c>
+      <c r="L442" s="8">
+        <v>-0.99</v>
+      </c>
+      <c r="M442" s="8">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="N442" s="8">
+        <v>0.43</v>
+      </c>
+      <c r="O442" s="7">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="443" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A443" s="10">
+        <v>44377</v>
+      </c>
+      <c r="B443" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C443" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="D443" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="E443" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="F443" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="H443" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="I443" s="8">
+        <v>1.03</v>
+      </c>
+      <c r="J443" s="8">
+        <v>1.76</v>
+      </c>
+      <c r="L443" s="8">
+        <v>-0.89</v>
+      </c>
+      <c r="M443" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="N443" s="8">
+        <v>0.53</v>
+      </c>
+      <c r="O443" s="7">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="444" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A444" s="10">
+        <v>44408</v>
+      </c>
+      <c r="B444" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C444" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="D444" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="E444" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="F444" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="H444" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="I444" s="8">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="J444" s="8">
+        <v>1.59</v>
+      </c>
+      <c r="L444" s="8">
+        <v>-0.8</v>
+      </c>
+      <c r="M444" s="8">
+        <v>-0.1</v>
+      </c>
+      <c r="N444" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="O444" s="7">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="445" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A445" s="10">
+        <v>44439</v>
+      </c>
+      <c r="B445" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C445" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="D445" s="8">
+        <v>0.39</v>
+      </c>
+      <c r="E445" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="F445" s="8">
+        <v>0.54</v>
+      </c>
+      <c r="H445" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="I445" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="J445" s="8">
+        <v>1.65</v>
+      </c>
+      <c r="L445" s="8">
+        <v>-0.72</v>
+      </c>
+      <c r="M445" s="8">
+        <v>-0.19</v>
+      </c>
+      <c r="N445" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="O445" s="7">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="446" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A446" s="10">
+        <v>44469</v>
+      </c>
+      <c r="B446" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C446" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D446" s="8">
+        <v>0.38</v>
+      </c>
+      <c r="E446" s="8">
+        <v>0.48</v>
+      </c>
+      <c r="F446" s="8">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H446" s="8">
+        <v>1.02</v>
+      </c>
+      <c r="I446" s="8">
+        <v>1.52</v>
+      </c>
+      <c r="J446" s="8">
+        <v>1.87</v>
+      </c>
+      <c r="L446" s="8">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="M446" s="8">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="N446" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="O446" s="7">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="447" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A447" s="10">
+        <v>44500</v>
+      </c>
+      <c r="B447" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C447" s="8">
+        <v>0.38</v>
+      </c>
+      <c r="D447" s="8">
+        <v>0.54</v>
+      </c>
+      <c r="E447" s="8">
+        <v>0.62</v>
+      </c>
+      <c r="F447" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="G447" s="8">
+        <v>1.33</v>
+      </c>
+      <c r="H447" s="8">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="I447" s="8">
+        <v>1.79</v>
+      </c>
+      <c r="J447" s="8">
+        <v>2.21</v>
+      </c>
+      <c r="L447" s="8">
+        <v>-0.53</v>
+      </c>
+      <c r="M447" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="N447" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="O447" s="7">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="448" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A448" s="10">
+        <v>44530</v>
+      </c>
+      <c r="B448" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="C448" s="8">
+        <v>0.54</v>
+      </c>
+      <c r="D448" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="E448" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="F448" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="G448" s="8">
+        <v>1.58</v>
+      </c>
+      <c r="H448" s="8">
+        <v>2.02</v>
+      </c>
+      <c r="I448" s="8">
+        <v>2.33</v>
+      </c>
+      <c r="J448" s="8">
+        <v>2.57</v>
+      </c>
+      <c r="L448" s="8">
+        <v>-0.35</v>
+      </c>
+      <c r="M448" s="8">
+        <v>0.41</v>
+      </c>
+      <c r="N448" s="8">
+        <v>0.68</v>
+      </c>
+      <c r="O448" s="7">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="449" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A449" s="10">
+        <v>44561</v>
+      </c>
+      <c r="B449" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="C449" s="8">
+        <v>0.71</v>
+      </c>
+      <c r="D449" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="E449" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="F449" s="8">
+        <v>0.91</v>
+      </c>
+      <c r="G449" s="8">
+        <v>1.52</v>
+      </c>
+      <c r="H449" s="8">
+        <v>1.97</v>
+      </c>
+      <c r="I449" s="8">
+        <v>2.21</v>
+      </c>
+      <c r="J449" s="8">
+        <v>2.38</v>
+      </c>
+      <c r="L449" s="8">
+        <v>-0.5</v>
+      </c>
+      <c r="M449" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="N449" s="8">
+        <v>0.54</v>
+      </c>
+      <c r="O449" s="7">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="450" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A450" s="10">
+        <v>44592</v>
+      </c>
+      <c r="B450" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="C450" s="8">
+        <v>0.67</v>
+      </c>
+      <c r="D450" s="8">
+        <v>0.82</v>
+      </c>
+      <c r="E450" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="F450" s="8">
+        <v>1.03</v>
+      </c>
+      <c r="G450" s="8">
+        <v>1.6</v>
+      </c>
+      <c r="H450" s="8">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="I450" s="8">
+        <v>2.36</v>
+      </c>
+      <c r="J450" s="8">
+        <v>2.56</v>
+      </c>
+      <c r="L450" s="8">
+        <v>-0.33</v>
+      </c>
+      <c r="M450" s="8">
+        <v>0.42</v>
+      </c>
+      <c r="N450" s="8">
+        <v>0.72</v>
+      </c>
+      <c r="O450" s="7">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="451" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A451" s="10">
+        <v>44620</v>
+      </c>
+      <c r="B451" s="8">
+        <v>1</v>
+      </c>
+      <c r="C451" s="8">
+        <v>0.73</v>
+      </c>
+      <c r="D451" s="8">
+        <v>1</v>
+      </c>
+      <c r="E451" s="8">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F451" s="8">
+        <v>1.21</v>
+      </c>
+      <c r="G451" s="8">
+        <v>1.82</v>
+      </c>
+      <c r="H451" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="I451" s="8">
+        <v>2.58</v>
+      </c>
+      <c r="J451" s="8">
+        <v>2.74</v>
+      </c>
+      <c r="L451" s="8">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="M451" s="8">
+        <v>0.61</v>
+      </c>
+      <c r="N451" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="O451" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A452" s="10">
+        <v>44651</v>
+      </c>
+      <c r="B452" s="8">
+        <v>1</v>
+      </c>
+      <c r="C452" s="8">
+        <v>0.94</v>
+      </c>
+      <c r="D452" s="8">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="E452" s="8">
+        <v>1.31</v>
+      </c>
+      <c r="F452" s="8">
+        <v>1.49</v>
+      </c>
+      <c r="G452" s="8">
+        <v>2.14</v>
+      </c>
+      <c r="H452" s="8">
+        <v>2.64</v>
+      </c>
+      <c r="I452" s="8">
+        <v>2.93</v>
+      </c>
+      <c r="J452" s="8">
+        <v>3.07</v>
+      </c>
+      <c r="L452" s="8">
+        <v>-0.17</v>
+      </c>
+      <c r="M452" s="8">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="N452" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="O452" s="7">
+        <v>0.91</v>
       </c>
     </row>
   </sheetData>
@@ -15418,7 +16136,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="9">
-        <v>44137</v>
+        <v>44652</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>